<commit_message>
add correlation matrix, run regressions, generate tables
</commit_message>
<xml_diff>
--- a/clean_data/new_data.xlsx
+++ b/clean_data/new_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/monicachang/Documents*/classes/spring 2021/GOV 94OA/research project/gilens-extension/clean_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1A3E0F-F907-564D-8ED9-B948A5B4D311}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F2E38F-3BF4-9A43-82E1-91B1C3798DE8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16080" xr2:uid="{27CBF91A-5F04-1440-B2EC-E3E89A09E45C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="209">
   <si>
     <t>switcher</t>
   </si>
@@ -656,13 +656,19 @@
   </si>
   <si>
     <t>inc12_dk</t>
+  </si>
+  <si>
+    <t>budget_reconciliation</t>
+  </si>
+  <si>
+    <t>filibuster_proof</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1038,17 +1044,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D314C2E4-4D75-2849-A6D8-BCEFC95C1EE9}">
-  <dimension ref="A1:AP153"/>
+  <dimension ref="A1:AR153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="82" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="F1" sqref="F1:F1048576"/>
+      <selection pane="bottomLeft" activeCell="AQ51" sqref="AQ51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:42">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1175,8 +1181,14 @@
       <c r="AP1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:42">
+      <c r="AQ1" t="s">
+        <v>207</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B2">
         <v>2009</v>
       </c>
@@ -1237,8 +1249,14 @@
       <c r="AP2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:42">
+      <c r="AQ2">
+        <v>0</v>
+      </c>
+      <c r="AR2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>2009</v>
       </c>
@@ -1299,8 +1317,14 @@
       <c r="AP3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:42">
+      <c r="AQ3">
+        <v>0</v>
+      </c>
+      <c r="AR3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>2009</v>
       </c>
@@ -1352,8 +1376,14 @@
       <c r="AP4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:42">
+      <c r="AQ4">
+        <v>0</v>
+      </c>
+      <c r="AR4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>2009</v>
       </c>
@@ -1414,8 +1444,14 @@
       <c r="AP5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:42">
+      <c r="AQ5">
+        <v>0</v>
+      </c>
+      <c r="AR5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>2009</v>
       </c>
@@ -1476,8 +1512,14 @@
       <c r="AP6" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="7" spans="1:42">
+      <c r="AQ6">
+        <v>0</v>
+      </c>
+      <c r="AR6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>2009</v>
       </c>
@@ -1538,8 +1580,14 @@
       <c r="AP7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:42">
+      <c r="AQ7">
+        <v>0</v>
+      </c>
+      <c r="AR7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>2009</v>
       </c>
@@ -1600,8 +1648,14 @@
       <c r="AP8" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="9" spans="1:42">
+      <c r="AQ8">
+        <v>0</v>
+      </c>
+      <c r="AR8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>2009</v>
       </c>
@@ -1662,8 +1716,14 @@
       <c r="AP9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:42">
+      <c r="AQ9">
+        <v>0</v>
+      </c>
+      <c r="AR9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>2009</v>
       </c>
@@ -1724,8 +1784,14 @@
       <c r="AP10" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="11" spans="1:42">
+      <c r="AQ10">
+        <v>0</v>
+      </c>
+      <c r="AR10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>2009</v>
       </c>
@@ -1786,8 +1852,14 @@
       <c r="AP11" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="1:42">
+      <c r="AQ11">
+        <v>0</v>
+      </c>
+      <c r="AR11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>2009</v>
       </c>
@@ -1848,8 +1920,14 @@
       <c r="AP12" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="13" spans="1:42">
+      <c r="AQ12">
+        <v>0</v>
+      </c>
+      <c r="AR12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>2009</v>
       </c>
@@ -1910,8 +1988,14 @@
       <c r="AP13" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="14" spans="1:42">
+      <c r="AQ13">
+        <v>0</v>
+      </c>
+      <c r="AR13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>2009</v>
       </c>
@@ -1972,8 +2056,14 @@
       <c r="AP14" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="15" spans="1:42">
+      <c r="AQ14">
+        <v>0</v>
+      </c>
+      <c r="AR14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B15">
         <v>2009</v>
       </c>
@@ -2034,8 +2124,14 @@
       <c r="AP15" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="16" spans="1:42">
+      <c r="AQ15">
+        <v>0</v>
+      </c>
+      <c r="AR15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B16">
         <v>2009</v>
       </c>
@@ -2096,8 +2192,14 @@
       <c r="AP16" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="17" spans="2:42">
+      <c r="AQ16">
+        <v>0</v>
+      </c>
+      <c r="AR16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B17">
         <v>2009</v>
       </c>
@@ -2131,8 +2233,14 @@
       <c r="AP17" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="18" spans="2:42">
+      <c r="AQ17">
+        <v>0</v>
+      </c>
+      <c r="AR17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>2009</v>
       </c>
@@ -2190,8 +2298,14 @@
       <c r="AP18" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="19" spans="2:42">
+      <c r="AQ18">
+        <v>0</v>
+      </c>
+      <c r="AR18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B19">
         <v>2009</v>
       </c>
@@ -2225,8 +2339,14 @@
       <c r="AP19" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="20" spans="2:42">
+      <c r="AQ19">
+        <v>0</v>
+      </c>
+      <c r="AR19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B20">
         <v>2009</v>
       </c>
@@ -2260,8 +2380,14 @@
       <c r="AP20" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="21" spans="2:42">
+      <c r="AQ20">
+        <v>0</v>
+      </c>
+      <c r="AR20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B21">
         <v>2009</v>
       </c>
@@ -2322,8 +2448,14 @@
       <c r="AP21" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="22" spans="2:42">
+      <c r="AQ21">
+        <v>0</v>
+      </c>
+      <c r="AR21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B22">
         <v>2009</v>
       </c>
@@ -2381,8 +2513,14 @@
       <c r="AP22" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="23" spans="2:42">
+      <c r="AQ22">
+        <v>0</v>
+      </c>
+      <c r="AR22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B23">
         <v>2009</v>
       </c>
@@ -2443,8 +2581,14 @@
       <c r="AP23" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="24" spans="2:42">
+      <c r="AQ23">
+        <v>0</v>
+      </c>
+      <c r="AR23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B24">
         <v>2009</v>
       </c>
@@ -2478,8 +2622,14 @@
       <c r="AP24" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="25" spans="2:42">
+      <c r="AQ24">
+        <v>0</v>
+      </c>
+      <c r="AR24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B25">
         <v>2009</v>
       </c>
@@ -2513,8 +2663,14 @@
       <c r="AP25" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="26" spans="2:42">
+      <c r="AQ25">
+        <v>1</v>
+      </c>
+      <c r="AR25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B26">
         <v>2009</v>
       </c>
@@ -2575,8 +2731,14 @@
       <c r="AP26" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="27" spans="2:42">
+      <c r="AQ26">
+        <v>0</v>
+      </c>
+      <c r="AR26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B27">
         <v>2009</v>
       </c>
@@ -2610,8 +2772,14 @@
       <c r="AP27" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="28" spans="2:42">
+      <c r="AQ27">
+        <v>0</v>
+      </c>
+      <c r="AR27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B28">
         <v>2009</v>
       </c>
@@ -2645,8 +2813,14 @@
       <c r="AP28" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="29" spans="2:42">
+      <c r="AQ28">
+        <v>1</v>
+      </c>
+      <c r="AR28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B29">
         <v>2009</v>
       </c>
@@ -2680,8 +2854,14 @@
       <c r="AP29" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="30" spans="2:42">
+      <c r="AQ29">
+        <v>1</v>
+      </c>
+      <c r="AR29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B30">
         <v>2009</v>
       </c>
@@ -2715,8 +2895,14 @@
       <c r="AP30" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="31" spans="2:42">
+      <c r="AQ30">
+        <v>0</v>
+      </c>
+      <c r="AR30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B31">
         <v>2009</v>
       </c>
@@ -2750,8 +2936,14 @@
       <c r="AP31" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="32" spans="2:42">
+      <c r="AQ31">
+        <v>0</v>
+      </c>
+      <c r="AR31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B32">
         <v>2009</v>
       </c>
@@ -2812,8 +3004,14 @@
       <c r="AP32" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="33" spans="2:42">
+      <c r="AQ32">
+        <v>0</v>
+      </c>
+      <c r="AR32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B33">
         <v>2009</v>
       </c>
@@ -2847,8 +3045,14 @@
       <c r="AP33" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="34" spans="2:42">
+      <c r="AQ33">
+        <v>1</v>
+      </c>
+      <c r="AR33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B34">
         <v>2009</v>
       </c>
@@ -2909,8 +3113,14 @@
       <c r="AP34" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="35" spans="2:42">
+      <c r="AQ34">
+        <v>0</v>
+      </c>
+      <c r="AR34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B35">
         <v>2009</v>
       </c>
@@ -2971,8 +3181,14 @@
       <c r="AP35" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="36" spans="2:42">
+      <c r="AQ35">
+        <v>0</v>
+      </c>
+      <c r="AR35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B36">
         <v>2009</v>
       </c>
@@ -3033,8 +3249,14 @@
       <c r="AP36" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="37" spans="2:42">
+      <c r="AQ36">
+        <v>0</v>
+      </c>
+      <c r="AR36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B37">
         <v>2010</v>
       </c>
@@ -3086,8 +3308,14 @@
       <c r="AP37" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="38" spans="2:42">
+      <c r="AQ37">
+        <v>0</v>
+      </c>
+      <c r="AR37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B38">
         <v>2010</v>
       </c>
@@ -3139,8 +3367,14 @@
       <c r="AP38" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="39" spans="2:42">
+      <c r="AQ38">
+        <v>0</v>
+      </c>
+      <c r="AR38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B39">
         <v>2010</v>
       </c>
@@ -3192,8 +3426,14 @@
       <c r="AP39" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="40" spans="2:42">
+      <c r="AQ39">
+        <v>0</v>
+      </c>
+      <c r="AR39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B40">
         <v>2010</v>
       </c>
@@ -3245,8 +3485,14 @@
       <c r="AP40" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="41" spans="2:42">
+      <c r="AQ40">
+        <v>0</v>
+      </c>
+      <c r="AR40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B41">
         <v>2010</v>
       </c>
@@ -3298,8 +3544,14 @@
       <c r="AP41" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="42" spans="2:42">
+      <c r="AQ41">
+        <v>0</v>
+      </c>
+      <c r="AR41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B42">
         <v>2010</v>
       </c>
@@ -3351,8 +3603,14 @@
       <c r="AP42" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="43" spans="2:42">
+      <c r="AQ42">
+        <v>0</v>
+      </c>
+      <c r="AR42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B43">
         <v>2010</v>
       </c>
@@ -3404,8 +3662,14 @@
       <c r="AP43" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="44" spans="2:42">
+      <c r="AQ43">
+        <v>0</v>
+      </c>
+      <c r="AR43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B44">
         <v>2010</v>
       </c>
@@ -3457,8 +3721,14 @@
       <c r="AP44" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="45" spans="2:42">
+      <c r="AQ44">
+        <v>1</v>
+      </c>
+      <c r="AR44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B45">
         <v>2010</v>
       </c>
@@ -3510,8 +3780,14 @@
       <c r="AP45" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="46" spans="2:42">
+      <c r="AQ45">
+        <v>0</v>
+      </c>
+      <c r="AR45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B46">
         <v>2010</v>
       </c>
@@ -3563,8 +3839,14 @@
       <c r="AP46" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="47" spans="2:42">
+      <c r="AQ46">
+        <v>0</v>
+      </c>
+      <c r="AR46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B47">
         <v>2010</v>
       </c>
@@ -3616,8 +3898,14 @@
       <c r="AP47" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="48" spans="2:42">
+      <c r="AQ47">
+        <v>0</v>
+      </c>
+      <c r="AR47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B48">
         <v>2010</v>
       </c>
@@ -3669,8 +3957,14 @@
       <c r="AP48" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="49" spans="2:42">
+      <c r="AQ48">
+        <v>1</v>
+      </c>
+      <c r="AR48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B49">
         <v>2010</v>
       </c>
@@ -3722,8 +4016,14 @@
       <c r="AP49" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="50" spans="2:42">
+      <c r="AQ49">
+        <v>0</v>
+      </c>
+      <c r="AR49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B50">
         <v>2010</v>
       </c>
@@ -3766,8 +4066,14 @@
       <c r="AP50" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="51" spans="2:42">
+      <c r="AQ50">
+        <v>0</v>
+      </c>
+      <c r="AR50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B51">
         <v>2010</v>
       </c>
@@ -3819,8 +4125,14 @@
       <c r="AP51" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="52" spans="2:42">
+      <c r="AQ51">
+        <v>0</v>
+      </c>
+      <c r="AR51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B52">
         <v>2010</v>
       </c>
@@ -3872,8 +4184,14 @@
       <c r="AP52" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="53" spans="2:42">
+      <c r="AQ52">
+        <v>0</v>
+      </c>
+      <c r="AR52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B53">
         <v>2010</v>
       </c>
@@ -3925,8 +4243,14 @@
       <c r="AP53" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="54" spans="2:42">
+      <c r="AQ53">
+        <v>0</v>
+      </c>
+      <c r="AR53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B54">
         <v>2010</v>
       </c>
@@ -3978,8 +4302,14 @@
       <c r="AP54" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="55" spans="2:42">
+      <c r="AQ54">
+        <v>0</v>
+      </c>
+      <c r="AR54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B55">
         <v>2010</v>
       </c>
@@ -4031,8 +4361,14 @@
       <c r="AP55" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="56" spans="2:42">
+      <c r="AQ55">
+        <v>0</v>
+      </c>
+      <c r="AR55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B56">
         <v>2010</v>
       </c>
@@ -4084,8 +4420,14 @@
       <c r="AP56" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="57" spans="2:42">
+      <c r="AQ56">
+        <v>0</v>
+      </c>
+      <c r="AR56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B57">
         <v>2010</v>
       </c>
@@ -4137,8 +4479,14 @@
       <c r="AP57" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="58" spans="2:42">
+      <c r="AQ57">
+        <v>0</v>
+      </c>
+      <c r="AR57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B58">
         <v>2010</v>
       </c>
@@ -4181,8 +4529,14 @@
       <c r="AP58" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="59" spans="2:42">
+      <c r="AQ58">
+        <v>0</v>
+      </c>
+      <c r="AR58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B59">
         <v>2010</v>
       </c>
@@ -4243,8 +4597,14 @@
       <c r="AP59" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="60" spans="2:42">
+      <c r="AQ59">
+        <v>0</v>
+      </c>
+      <c r="AR59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B60">
         <v>2010</v>
       </c>
@@ -4305,8 +4665,14 @@
       <c r="AP60" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="61" spans="2:42">
+      <c r="AQ60">
+        <v>0</v>
+      </c>
+      <c r="AR60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B61">
         <v>2010</v>
       </c>
@@ -4367,8 +4733,14 @@
       <c r="AP61" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="62" spans="2:42">
+      <c r="AQ61">
+        <v>0</v>
+      </c>
+      <c r="AR61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B62">
         <v>2010</v>
       </c>
@@ -4429,8 +4801,14 @@
       <c r="AP62" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="63" spans="2:42">
+      <c r="AQ62">
+        <v>0</v>
+      </c>
+      <c r="AR62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B63">
         <v>2010</v>
       </c>
@@ -4491,8 +4869,14 @@
       <c r="AP63" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="64" spans="2:42">
+      <c r="AQ63">
+        <v>0</v>
+      </c>
+      <c r="AR63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B64">
         <v>2010</v>
       </c>
@@ -4553,8 +4937,14 @@
       <c r="AP64" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="65" spans="2:42">
+      <c r="AQ64">
+        <v>0</v>
+      </c>
+      <c r="AR64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B65">
         <v>2010</v>
       </c>
@@ -4588,8 +4978,14 @@
       <c r="AP65" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="66" spans="2:42">
+      <c r="AQ65">
+        <v>0</v>
+      </c>
+      <c r="AR65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B66">
         <v>2010</v>
       </c>
@@ -4623,8 +5019,14 @@
       <c r="AP66" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="67" spans="2:42">
+      <c r="AQ66">
+        <v>0</v>
+      </c>
+      <c r="AR66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B67">
         <v>2010</v>
       </c>
@@ -4658,8 +5060,14 @@
       <c r="AP67" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="68" spans="2:42">
+      <c r="AQ67">
+        <v>0</v>
+      </c>
+      <c r="AR67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B68">
         <v>2010</v>
       </c>
@@ -4693,8 +5101,14 @@
       <c r="AP68" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="69" spans="2:42">
+      <c r="AQ68">
+        <v>0</v>
+      </c>
+      <c r="AR68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B69">
         <v>2010</v>
       </c>
@@ -4728,8 +5142,14 @@
       <c r="AP69" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="70" spans="2:42">
+      <c r="AQ69">
+        <v>0</v>
+      </c>
+      <c r="AR69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B70">
         <v>2010</v>
       </c>
@@ -4763,8 +5183,14 @@
       <c r="AP70" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="71" spans="2:42">
+      <c r="AQ70">
+        <v>0</v>
+      </c>
+      <c r="AR70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B71">
         <v>2010</v>
       </c>
@@ -4825,8 +5251,14 @@
       <c r="AP71" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="72" spans="2:42">
+      <c r="AQ71">
+        <v>0</v>
+      </c>
+      <c r="AR71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B72">
         <v>2010</v>
       </c>
@@ -4887,8 +5319,14 @@
       <c r="AP72" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="73" spans="2:42">
+      <c r="AQ72">
+        <v>0</v>
+      </c>
+      <c r="AR72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B73">
         <v>2010</v>
       </c>
@@ -4949,8 +5387,14 @@
       <c r="AP73" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="74" spans="2:42">
+      <c r="AQ73">
+        <v>0</v>
+      </c>
+      <c r="AR73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B74">
         <v>2010</v>
       </c>
@@ -5011,8 +5455,14 @@
       <c r="AP74" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="75" spans="2:42">
+      <c r="AQ74">
+        <v>0</v>
+      </c>
+      <c r="AR74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B75">
         <v>2010</v>
       </c>
@@ -5073,8 +5523,14 @@
       <c r="AP75" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="76" spans="2:42">
+      <c r="AQ75">
+        <v>0</v>
+      </c>
+      <c r="AR75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B76">
         <v>2010</v>
       </c>
@@ -5135,8 +5591,14 @@
       <c r="AP76" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="77" spans="2:42">
+      <c r="AQ76">
+        <v>0</v>
+      </c>
+      <c r="AR76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B77">
         <v>2010</v>
       </c>
@@ -5197,8 +5659,14 @@
       <c r="AP77" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="78" spans="2:42">
+      <c r="AQ77">
+        <v>0</v>
+      </c>
+      <c r="AR77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B78">
         <v>2010</v>
       </c>
@@ -5259,8 +5727,14 @@
       <c r="AP78" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="79" spans="2:42">
+      <c r="AQ78">
+        <v>0</v>
+      </c>
+      <c r="AR78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B79">
         <v>2011</v>
       </c>
@@ -5312,8 +5786,14 @@
       <c r="AP79" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="80" spans="2:42">
+      <c r="AQ79">
+        <v>0</v>
+      </c>
+      <c r="AR79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B80">
         <v>2011</v>
       </c>
@@ -5365,8 +5845,14 @@
       <c r="AP80" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="81" spans="2:42">
+      <c r="AQ80">
+        <v>0</v>
+      </c>
+      <c r="AR80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B81">
         <v>2011</v>
       </c>
@@ -5418,8 +5904,14 @@
       <c r="AP81" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="82" spans="2:42">
+      <c r="AQ81">
+        <v>0</v>
+      </c>
+      <c r="AR81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B82">
         <v>2011</v>
       </c>
@@ -5471,8 +5963,14 @@
       <c r="AP82" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="83" spans="2:42">
+      <c r="AQ82">
+        <v>0</v>
+      </c>
+      <c r="AR82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B83">
         <v>2011</v>
       </c>
@@ -5524,8 +6022,14 @@
       <c r="AP83" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="84" spans="2:42">
+      <c r="AQ83">
+        <v>0</v>
+      </c>
+      <c r="AR83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B84">
         <v>2011</v>
       </c>
@@ -5577,8 +6081,14 @@
       <c r="AP84" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="85" spans="2:42">
+      <c r="AQ84">
+        <v>0</v>
+      </c>
+      <c r="AR84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B85">
         <v>2011</v>
       </c>
@@ -5630,8 +6140,14 @@
       <c r="AP85" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="86" spans="2:42">
+      <c r="AQ85">
+        <v>0</v>
+      </c>
+      <c r="AR85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B86">
         <v>2011</v>
       </c>
@@ -5683,8 +6199,14 @@
       <c r="AP86" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="87" spans="2:42">
+      <c r="AQ86">
+        <v>0</v>
+      </c>
+      <c r="AR86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B87">
         <v>2011</v>
       </c>
@@ -5736,8 +6258,14 @@
       <c r="AP87" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="88" spans="2:42">
+      <c r="AQ87">
+        <v>0</v>
+      </c>
+      <c r="AR87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B88">
         <v>2011</v>
       </c>
@@ -5789,8 +6317,14 @@
       <c r="AP88" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="89" spans="2:42">
+      <c r="AQ88">
+        <v>0</v>
+      </c>
+      <c r="AR88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B89">
         <v>2011</v>
       </c>
@@ -5842,8 +6376,14 @@
       <c r="AP89" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="90" spans="2:42">
+      <c r="AQ89">
+        <v>0</v>
+      </c>
+      <c r="AR89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B90">
         <v>2011</v>
       </c>
@@ -5895,8 +6435,14 @@
       <c r="AP90" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="91" spans="2:42">
+      <c r="AQ90">
+        <v>0</v>
+      </c>
+      <c r="AR90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B91">
         <v>2011</v>
       </c>
@@ -5948,8 +6494,14 @@
       <c r="AP91" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="92" spans="2:42">
+      <c r="AQ91">
+        <v>0</v>
+      </c>
+      <c r="AR91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B92">
         <v>2011</v>
       </c>
@@ -6001,8 +6553,14 @@
       <c r="AP92" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="93" spans="2:42">
+      <c r="AQ92">
+        <v>0</v>
+      </c>
+      <c r="AR92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B93">
         <v>2011</v>
       </c>
@@ -6054,8 +6612,14 @@
       <c r="AP93" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="94" spans="2:42">
+      <c r="AQ93">
+        <v>0</v>
+      </c>
+      <c r="AR93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B94">
         <v>2011</v>
       </c>
@@ -6107,8 +6671,14 @@
       <c r="AP94" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="95" spans="2:42">
+      <c r="AQ94">
+        <v>0</v>
+      </c>
+      <c r="AR94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B95">
         <v>2011</v>
       </c>
@@ -6169,8 +6739,14 @@
       <c r="AP95" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="96" spans="2:42">
+      <c r="AQ95">
+        <v>0</v>
+      </c>
+      <c r="AR95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B96">
         <v>2011</v>
       </c>
@@ -6231,8 +6807,14 @@
       <c r="AP96" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="97" spans="2:42">
+      <c r="AQ96">
+        <v>0</v>
+      </c>
+      <c r="AR96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B97">
         <v>2011</v>
       </c>
@@ -6284,8 +6866,14 @@
       <c r="AP97" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="98" spans="2:42">
+      <c r="AQ97">
+        <v>0</v>
+      </c>
+      <c r="AR97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B98">
         <v>2011</v>
       </c>
@@ -6337,8 +6925,14 @@
       <c r="AP98" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="99" spans="2:42">
+      <c r="AQ98">
+        <v>0</v>
+      </c>
+      <c r="AR98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B99">
         <v>2011</v>
       </c>
@@ -6390,8 +6984,14 @@
       <c r="AP99" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="100" spans="2:42">
+      <c r="AQ99">
+        <v>0</v>
+      </c>
+      <c r="AR99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B100">
         <v>2011</v>
       </c>
@@ -6443,8 +7043,14 @@
       <c r="AP100" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="101" spans="2:42">
+      <c r="AQ100">
+        <v>0</v>
+      </c>
+      <c r="AR100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B101">
         <v>2011</v>
       </c>
@@ -6496,8 +7102,14 @@
       <c r="AP101" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="102" spans="2:42">
+      <c r="AQ101">
+        <v>0</v>
+      </c>
+      <c r="AR101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B102">
         <v>2011</v>
       </c>
@@ -6549,8 +7161,14 @@
       <c r="AP102" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="103" spans="2:42">
+      <c r="AQ102">
+        <v>0</v>
+      </c>
+      <c r="AR102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B103">
         <v>2011</v>
       </c>
@@ -6602,8 +7220,14 @@
       <c r="AP103" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="104" spans="2:42">
+      <c r="AQ103">
+        <v>0</v>
+      </c>
+      <c r="AR103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B104">
         <v>2011</v>
       </c>
@@ -6655,8 +7279,14 @@
       <c r="AP104" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="105" spans="2:42">
+      <c r="AQ104">
+        <v>0</v>
+      </c>
+      <c r="AR104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B105">
         <v>2011</v>
       </c>
@@ -6708,8 +7338,14 @@
       <c r="AP105" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="106" spans="2:42">
+      <c r="AQ105">
+        <v>0</v>
+      </c>
+      <c r="AR105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B106">
         <v>2011</v>
       </c>
@@ -6761,8 +7397,14 @@
       <c r="AP106" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="107" spans="2:42">
+      <c r="AQ106">
+        <v>0</v>
+      </c>
+      <c r="AR106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B107">
         <v>2011</v>
       </c>
@@ -6814,8 +7456,14 @@
       <c r="AP107" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="108" spans="2:42">
+      <c r="AQ107">
+        <v>0</v>
+      </c>
+      <c r="AR107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B108">
         <v>2011</v>
       </c>
@@ -6867,8 +7515,14 @@
       <c r="AP108" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="109" spans="2:42">
+      <c r="AQ108">
+        <v>0</v>
+      </c>
+      <c r="AR108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B109">
         <v>2011</v>
       </c>
@@ -6920,8 +7574,14 @@
       <c r="AP109" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="110" spans="2:42">
+      <c r="AQ109">
+        <v>0</v>
+      </c>
+      <c r="AR109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B110">
         <v>2011</v>
       </c>
@@ -6973,8 +7633,14 @@
       <c r="AP110" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="111" spans="2:42">
+      <c r="AQ110">
+        <v>0</v>
+      </c>
+      <c r="AR110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B111">
         <v>2011</v>
       </c>
@@ -7026,8 +7692,14 @@
       <c r="AP111" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="112" spans="2:42">
+      <c r="AQ111">
+        <v>0</v>
+      </c>
+      <c r="AR111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B112">
         <v>2011</v>
       </c>
@@ -7079,8 +7751,14 @@
       <c r="AP112" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="113" spans="2:42">
+      <c r="AQ112">
+        <v>0</v>
+      </c>
+      <c r="AR112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B113">
         <v>2011</v>
       </c>
@@ -7132,8 +7810,14 @@
       <c r="AP113" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="114" spans="2:42">
+      <c r="AQ113">
+        <v>0</v>
+      </c>
+      <c r="AR113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B114">
         <v>2011</v>
       </c>
@@ -7185,8 +7869,14 @@
       <c r="AP114" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="115" spans="2:42">
+      <c r="AQ114">
+        <v>0</v>
+      </c>
+      <c r="AR114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B115">
         <v>2011</v>
       </c>
@@ -7238,8 +7928,14 @@
       <c r="AP115" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="116" spans="2:42">
+      <c r="AQ115">
+        <v>0</v>
+      </c>
+      <c r="AR115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B116">
         <v>2011</v>
       </c>
@@ -7291,8 +7987,14 @@
       <c r="AP116" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="117" spans="2:42">
+      <c r="AQ116">
+        <v>0</v>
+      </c>
+      <c r="AR116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B117">
         <v>2011</v>
       </c>
@@ -7344,8 +8046,14 @@
       <c r="AP117" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="118" spans="2:42">
+      <c r="AQ117">
+        <v>0</v>
+      </c>
+      <c r="AR117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B118">
         <v>2011</v>
       </c>
@@ -7397,8 +8105,14 @@
       <c r="AP118" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="119" spans="2:42">
+      <c r="AQ118">
+        <v>0</v>
+      </c>
+      <c r="AR118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B119">
         <v>2011</v>
       </c>
@@ -7450,8 +8164,14 @@
       <c r="AP119" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="120" spans="2:42">
+      <c r="AQ119">
+        <v>0</v>
+      </c>
+      <c r="AR119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B120">
         <v>2011</v>
       </c>
@@ -7503,8 +8223,14 @@
       <c r="AP120" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="121" spans="2:42">
+      <c r="AQ120">
+        <v>0</v>
+      </c>
+      <c r="AR120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B121">
         <v>2011</v>
       </c>
@@ -7556,8 +8282,14 @@
       <c r="AP121" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="122" spans="2:42">
+      <c r="AQ121">
+        <v>0</v>
+      </c>
+      <c r="AR121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B122">
         <v>2012</v>
       </c>
@@ -7609,8 +8341,14 @@
       <c r="AP122" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="123" spans="2:42">
+      <c r="AQ122">
+        <v>0</v>
+      </c>
+      <c r="AR122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B123">
         <v>2012</v>
       </c>
@@ -7662,8 +8400,14 @@
       <c r="AP123" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="124" spans="2:42">
+      <c r="AQ123">
+        <v>0</v>
+      </c>
+      <c r="AR123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B124">
         <v>2012</v>
       </c>
@@ -7706,8 +8450,14 @@
       <c r="AP124" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="125" spans="2:42">
+      <c r="AQ124">
+        <v>0</v>
+      </c>
+      <c r="AR124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B125">
         <v>2012</v>
       </c>
@@ -7759,8 +8509,14 @@
       <c r="AP125" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="126" spans="2:42">
+      <c r="AQ125">
+        <v>0</v>
+      </c>
+      <c r="AR125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B126">
         <v>2012</v>
       </c>
@@ -7812,8 +8568,14 @@
       <c r="AP126" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="127" spans="2:42">
+      <c r="AQ126">
+        <v>0</v>
+      </c>
+      <c r="AR126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B127">
         <v>2012</v>
       </c>
@@ -7865,8 +8627,14 @@
       <c r="AP127" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="128" spans="2:42">
+      <c r="AQ127">
+        <v>0</v>
+      </c>
+      <c r="AR127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B128">
         <v>2012</v>
       </c>
@@ -7918,8 +8686,14 @@
       <c r="AP128" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="129" spans="2:42">
+      <c r="AQ128">
+        <v>0</v>
+      </c>
+      <c r="AR128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B129">
         <v>2012</v>
       </c>
@@ -7971,8 +8745,14 @@
       <c r="AP129" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="130" spans="2:42">
+      <c r="AQ129">
+        <v>0</v>
+      </c>
+      <c r="AR129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B130">
         <v>2012</v>
       </c>
@@ -8024,8 +8804,14 @@
       <c r="AP130" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="131" spans="2:42">
+      <c r="AQ130">
+        <v>0</v>
+      </c>
+      <c r="AR130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B131">
         <v>2012</v>
       </c>
@@ -8077,8 +8863,14 @@
       <c r="AP131" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="132" spans="2:42">
+      <c r="AQ131">
+        <v>0</v>
+      </c>
+      <c r="AR131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B132">
         <v>2012</v>
       </c>
@@ -8130,8 +8922,14 @@
       <c r="AP132" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="133" spans="2:42">
+      <c r="AQ132">
+        <v>0</v>
+      </c>
+      <c r="AR132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B133">
         <v>2012</v>
       </c>
@@ -8183,8 +8981,14 @@
       <c r="AP133" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="134" spans="2:42">
+      <c r="AQ133">
+        <v>0</v>
+      </c>
+      <c r="AR133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B134">
         <v>2012</v>
       </c>
@@ -8236,8 +9040,14 @@
       <c r="AP134" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="135" spans="2:42">
+      <c r="AQ134">
+        <v>0</v>
+      </c>
+      <c r="AR134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B135">
         <v>2012</v>
       </c>
@@ -8289,8 +9099,14 @@
       <c r="AP135" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="136" spans="2:42">
+      <c r="AQ135">
+        <v>0</v>
+      </c>
+      <c r="AR135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B136">
         <v>2012</v>
       </c>
@@ -8342,8 +9158,14 @@
       <c r="AP136" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="137" spans="2:42">
+      <c r="AQ136">
+        <v>0</v>
+      </c>
+      <c r="AR136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B137">
         <v>2012</v>
       </c>
@@ -8395,8 +9217,14 @@
       <c r="AP137" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="138" spans="2:42">
+      <c r="AQ137">
+        <v>0</v>
+      </c>
+      <c r="AR137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B138">
         <v>2013</v>
       </c>
@@ -8448,8 +9276,14 @@
       <c r="AP138" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="139" spans="2:42">
+      <c r="AQ138">
+        <v>0</v>
+      </c>
+      <c r="AR138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B139">
         <v>2013</v>
       </c>
@@ -8501,8 +9335,14 @@
       <c r="AP139" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="140" spans="2:42">
+      <c r="AQ139">
+        <v>0</v>
+      </c>
+      <c r="AR139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B140">
         <v>2013</v>
       </c>
@@ -8554,8 +9394,14 @@
       <c r="AP140" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="141" spans="2:42">
+      <c r="AQ140">
+        <v>0</v>
+      </c>
+      <c r="AR140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B141">
         <v>2013</v>
       </c>
@@ -8607,8 +9453,14 @@
       <c r="AP141" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="142" spans="2:42">
+      <c r="AQ141">
+        <v>0</v>
+      </c>
+      <c r="AR141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B142">
         <v>2013</v>
       </c>
@@ -8660,8 +9512,14 @@
       <c r="AP142" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="143" spans="2:42">
+      <c r="AQ142">
+        <v>0</v>
+      </c>
+      <c r="AR142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B143">
         <v>2013</v>
       </c>
@@ -8713,8 +9571,14 @@
       <c r="AP143" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="144" spans="2:42">
+      <c r="AQ143">
+        <v>0</v>
+      </c>
+      <c r="AR143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B144">
         <v>2013</v>
       </c>
@@ -8772,8 +9636,14 @@
       <c r="AP144" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="145" spans="2:42">
+      <c r="AQ144">
+        <v>0</v>
+      </c>
+      <c r="AR144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B145">
         <v>2013</v>
       </c>
@@ -8825,8 +9695,14 @@
       <c r="AP145" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="146" spans="2:42">
+      <c r="AQ145">
+        <v>0</v>
+      </c>
+      <c r="AR145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B146">
         <v>2013</v>
       </c>
@@ -8878,8 +9754,14 @@
       <c r="AP146" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="147" spans="2:42">
+      <c r="AQ146">
+        <v>0</v>
+      </c>
+      <c r="AR146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B147">
         <v>2013</v>
       </c>
@@ -8931,8 +9813,14 @@
       <c r="AP147" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="148" spans="2:42">
+      <c r="AQ147">
+        <v>0</v>
+      </c>
+      <c r="AR147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B148">
         <v>2013</v>
       </c>
@@ -8984,8 +9872,14 @@
       <c r="AP148" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="149" spans="2:42">
+      <c r="AQ148">
+        <v>0</v>
+      </c>
+      <c r="AR148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B149">
         <v>2013</v>
       </c>
@@ -9037,8 +9931,14 @@
       <c r="AP149" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="150" spans="2:42">
+      <c r="AQ149">
+        <v>0</v>
+      </c>
+      <c r="AR149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B150">
         <v>2013</v>
       </c>
@@ -9090,8 +9990,14 @@
       <c r="AP150" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="151" spans="2:42">
+      <c r="AQ150">
+        <v>0</v>
+      </c>
+      <c r="AR150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B151">
         <v>2013</v>
       </c>
@@ -9143,8 +10049,14 @@
       <c r="AP151" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="152" spans="2:42">
+      <c r="AQ151">
+        <v>0</v>
+      </c>
+      <c r="AR151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B152">
         <v>2013</v>
       </c>
@@ -9196,8 +10108,14 @@
       <c r="AP152" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="153" spans="2:42">
+      <c r="AQ152">
+        <v>0</v>
+      </c>
+      <c r="AR152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B153">
         <v>2013</v>
       </c>
@@ -9248,6 +10166,12 @@
       </c>
       <c r="AP153" t="s">
         <v>185</v>
+      </c>
+      <c r="AQ153">
+        <v>0</v>
+      </c>
+      <c r="AR153">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -9263,24 +10187,24 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="28">
+    <row r="3" spans="1:1" ht="28" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>116</v>
       </c>

</xml_diff>